<commit_message>
updated materials.xlsx, schematic.pptx & multithreaded code (might not be needed though, the single core code worked better than expected). added datasheet for gearbox motor.
</commit_message>
<xml_diff>
--- a/materials.xlsx
+++ b/materials.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samik\Documents\Koulu\digitaalisen_valmistuksen_perusteet\group23\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{238E3E72-F438-4E3F-961C-5D0409948E84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C682126C-5C8E-4729-B6DC-3BE9FB36E501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{206C7778-B294-4357-AFEA-16B3EFD6E54B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{206C7778-B294-4357-AFEA-16B3EFD6E54B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="75">
   <si>
     <t>Materials</t>
   </si>
@@ -125,9 +125,6 @@
     <t>Gear motor</t>
   </si>
   <si>
-    <t>link or something??</t>
-  </si>
-  <si>
     <t>H-bridge</t>
   </si>
   <si>
@@ -173,9 +170,6 @@
     <t>4??</t>
   </si>
   <si>
-    <t>so many</t>
-  </si>
-  <si>
     <t>max. 1 roll :D</t>
   </si>
   <si>
@@ -231,6 +225,42 @@
   </si>
   <si>
     <t>M4??</t>
+  </si>
+  <si>
+    <t>GEARMOTOR 200 RPM 3-6V DC (Adafruit 3777??)</t>
+  </si>
+  <si>
+    <t>link or something?? Markings on the bag??</t>
+  </si>
+  <si>
+    <t>?? Markings on the bag??</t>
+  </si>
+  <si>
+    <t>35931.574 mm3</t>
+  </si>
+  <si>
+    <t>9002.649 mm3</t>
+  </si>
+  <si>
+    <t>9213.417 mm3</t>
+  </si>
+  <si>
+    <t>?? Which one??</t>
+  </si>
+  <si>
+    <t>(brackets for not yet implemented/ready components/materials)</t>
+  </si>
+  <si>
+    <t>remember to add jumpers with power source</t>
+  </si>
+  <si>
+    <t>+ 3 male-female</t>
+  </si>
+  <si>
+    <t>+ 2 female-female</t>
+  </si>
+  <si>
+    <t>maybe</t>
   </si>
 </sst>
 </file>
@@ -531,7 +561,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -554,6 +584,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -888,10 +919,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11BCCBEE-3478-41B5-8E92-3DF53108FB7E}">
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -900,7 +931,7 @@
     <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
@@ -918,10 +949,10 @@
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E3">
-        <v>250418</v>
+        <v>250420</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -984,7 +1015,7 @@
         <v>10</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="D8" s="6">
         <v>2</v>
@@ -1001,7 +1032,7 @@
         <v>16</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>11</v>
+        <v>68</v>
       </c>
       <c r="D9" s="6">
         <v>1</v>
@@ -1018,7 +1049,7 @@
         <v>17</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>11</v>
+        <v>67</v>
       </c>
       <c r="D10" s="6">
         <v>2</v>
@@ -1114,7 +1145,7 @@
         <v>2</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>29</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1122,14 +1153,14 @@
         <v>12</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="6">
         <v>1</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1137,14 +1168,14 @@
         <v>13</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="6">
         <v>1</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1152,14 +1183,14 @@
         <v>14</v>
       </c>
       <c r="B19" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6">
+        <v>17</v>
+      </c>
+      <c r="E19" s="18" t="s">
         <v>34</v>
-      </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E19" s="18" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1167,14 +1198,14 @@
         <v>15</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C20" s="6"/>
-      <c r="D20" s="6" t="s">
-        <v>44</v>
+      <c r="D20" s="6">
+        <v>6</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1182,14 +1213,14 @@
         <v>16</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="6">
         <v>2</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1197,14 +1228,14 @@
         <v>17</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="6">
         <v>1</v>
       </c>
       <c r="E22" s="18" t="s">
-        <v>6</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1212,14 +1243,14 @@
         <v>18</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="6">
         <v>1</v>
       </c>
       <c r="E23" s="18" t="s">
-        <v>6</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1227,14 +1258,14 @@
         <v>19</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="6">
         <v>1</v>
       </c>
       <c r="E24" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1242,14 +1273,14 @@
         <v>20</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C25" s="6"/>
       <c r="D25" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E25" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1257,7 +1288,7 @@
         <v>21</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>11</v>
@@ -1266,7 +1297,7 @@
         <v>2</v>
       </c>
       <c r="E26" s="18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1274,7 +1305,7 @@
         <v>22</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>11</v>
@@ -1291,7 +1322,7 @@
         <v>23</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>11</v>
@@ -1300,7 +1331,7 @@
         <v>1</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1308,7 +1339,7 @@
         <v>24</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>6</v>
@@ -1317,7 +1348,7 @@
         <v>1</v>
       </c>
       <c r="E29" s="18" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1325,14 +1356,14 @@
         <v>25</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C30" s="6"/>
       <c r="D30" s="6">
         <v>2</v>
       </c>
       <c r="E30" s="18" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1340,14 +1371,14 @@
         <v>26</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C31" s="6"/>
       <c r="D31" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E31" s="18" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1355,14 +1386,14 @@
         <v>27</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C32" s="6"/>
       <c r="D32" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E32" s="18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1370,7 +1401,7 @@
         <v>28</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C33" s="6"/>
       <c r="D33" s="6" t="s">
@@ -1385,7 +1416,7 @@
         <v>29</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C34" s="6"/>
       <c r="D34" s="6" t="s">
@@ -1400,7 +1431,7 @@
         <v>30</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C35" s="6"/>
       <c r="D35" s="6" t="s">
@@ -1500,7 +1531,227 @@
       <c r="D45" s="20"/>
       <c r="E45" s="21"/>
     </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B50" s="22" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51" s="22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>74</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Asiakirja" ma:contentTypeID="0x010100288FF80C09CDD44CBEDCB6BDA3BB791A" ma:contentTypeVersion="3" ma:contentTypeDescription="Luo uusi asiakirja." ma:contentTypeScope="" ma:versionID="e4c01c7c4b2fa601b9adbc8cdf8d23de">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="da167cd1-d7a6-4338-bc63-7a91f955c7fa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="30409ac8fa297c07eb11085401007006" ns2:_="">
+    <xsd:import namespace="da167cd1-d7a6-4338-bc63-7a91f955c7fa"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="da167cd1-d7a6-4338-bc63-7a91f955c7fa" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="10" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Sisältölaji"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Otsikko"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0738F08B-BAB3-4861-8EE3-0808A07B6694}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="da167cd1-d7a6-4338-bc63-7a91f955c7fa"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{884C2661-2447-498C-AC3E-3E7F14D4616E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CE5D208-A7B2-407E-BE4C-99D8E137B990}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="da167cd1-d7a6-4338-bc63-7a91f955c7fa"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated materials.xlsx with draft costs
</commit_message>
<xml_diff>
--- a/materials.xlsx
+++ b/materials.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samik\Documents\Koulu\digitaalisen_valmistuksen_perusteet\group23\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C682126C-5C8E-4729-B6DC-3BE9FB36E501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71940496-3A5C-49BC-9770-DEA8F0B78090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{206C7778-B294-4357-AFEA-16B3EFD6E54B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{206C7778-B294-4357-AFEA-16B3EFD6E54B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="82">
   <si>
     <t>Materials</t>
   </si>
@@ -261,6 +261,27 @@
   </si>
   <si>
     <t>maybe</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>mm3</t>
+  </si>
+  <si>
+    <t>piece</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Cost per unit [€]</t>
+  </si>
+  <si>
+    <t>Total [€]</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
   </si>
 </sst>
 </file>
@@ -325,7 +346,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -407,37 +428,13 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -450,7 +447,9 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -466,7 +465,100 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -475,7 +567,50 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -490,13 +625,13 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -509,59 +644,14 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -572,19 +662,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -919,10 +1019,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11BCCBEE-3478-41B5-8E92-3DF53108FB7E}">
-  <dimension ref="A1:E52"/>
+  <dimension ref="A1:H52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -932,19 +1032,20 @@
     <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="43.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -952,15 +1053,15 @@
         <v>54</v>
       </c>
       <c r="E3">
-        <v>250420</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="13" t="s">
+        <v>250423</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="22" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="8" t="s">
@@ -969,15 +1070,24 @@
       <c r="D5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="18" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="14">
+      <c r="F5" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="G5" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="H5" s="24" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="11">
         <v>1</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="25" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="7" t="s">
@@ -986,15 +1096,20 @@
       <c r="D6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="19" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="15">
+      <c r="F6" s="7"/>
+      <c r="G6" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="H6" s="14"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="12">
         <v>2</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="26" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="6" t="s">
@@ -1003,15 +1118,20 @@
       <c r="D7" s="6">
         <v>2</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="20" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="15">
+      <c r="F7" s="6"/>
+      <c r="G7" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="H7" s="15"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="12">
         <v>3</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="26" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="6" t="s">
@@ -1020,15 +1140,20 @@
       <c r="D8" s="6">
         <v>2</v>
       </c>
-      <c r="E8" s="18" t="s">
+      <c r="E8" s="20" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="15">
+      <c r="F8" s="6"/>
+      <c r="G8" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="H8" s="15"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="12">
         <v>4</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="26" t="s">
         <v>16</v>
       </c>
       <c r="C9" s="6" t="s">
@@ -1037,15 +1162,20 @@
       <c r="D9" s="6">
         <v>1</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="20" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="15">
+      <c r="F9" s="6"/>
+      <c r="G9" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="H9" s="15"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="12">
         <v>5</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="26" t="s">
         <v>17</v>
       </c>
       <c r="C10" s="6" t="s">
@@ -1054,240 +1184,379 @@
       <c r="D10" s="6">
         <v>2</v>
       </c>
-      <c r="E10" s="18" t="s">
+      <c r="E10" s="20" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="15">
+      <c r="F10" s="6"/>
+      <c r="G10" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="H10" s="15"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="12">
         <v>6</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="26" t="s">
         <v>19</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6">
         <v>1</v>
       </c>
-      <c r="E11" s="18" t="s">
+      <c r="E11" s="20" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="15">
+      <c r="F11" s="6">
+        <v>8.11</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="H11" s="15">
+        <f>D11*F11</f>
+        <v>8.11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="12">
         <v>7</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="26" t="s">
         <v>21</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="6">
         <v>1</v>
       </c>
-      <c r="E12" s="18" t="s">
+      <c r="E12" s="20" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="15">
+      <c r="F12" s="6">
+        <v>5.35</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="H12" s="15">
+        <f t="shared" ref="H12:H20" si="0">D12*F12</f>
+        <v>5.35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="12">
         <v>8</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="26" t="s">
         <v>21</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6">
         <v>1</v>
       </c>
-      <c r="E13" s="18" t="s">
+      <c r="E13" s="20" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="15">
+      <c r="F13" s="6">
+        <v>2.72</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="H13" s="15">
+        <f t="shared" si="0"/>
+        <v>2.72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
         <v>9</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="26" t="s">
         <v>24</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6">
         <v>2</v>
       </c>
-      <c r="E14" s="18" t="s">
+      <c r="E14" s="20" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="15">
+      <c r="F14" s="6">
+        <v>0.46</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="H14" s="15">
+        <f t="shared" si="0"/>
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="12">
         <v>10</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="26" t="s">
         <v>26</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="6">
         <v>2</v>
       </c>
-      <c r="E15" s="18" t="s">
+      <c r="E15" s="20" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="15">
+      <c r="F15" s="6">
+        <v>0.24</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="H15" s="15">
+        <f t="shared" si="0"/>
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="12">
         <v>11</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="26" t="s">
         <v>28</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6">
         <v>2</v>
       </c>
-      <c r="E16" s="18" t="s">
+      <c r="E16" s="20" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="15">
+      <c r="F16" s="6">
+        <v>2.72</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="H16" s="15">
+        <f t="shared" si="0"/>
+        <v>5.44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="12">
         <v>12</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="26" t="s">
         <v>29</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="6">
         <v>1</v>
       </c>
-      <c r="E17" s="18" t="s">
+      <c r="E17" s="20" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="15">
+      <c r="F17" s="6">
+        <v>7.24</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="H17" s="15">
+        <f t="shared" si="0"/>
+        <v>7.24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="12">
         <v>13</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="26" t="s">
         <v>31</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="6">
         <v>1</v>
       </c>
-      <c r="E18" s="18" t="s">
+      <c r="E18" s="20" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="15">
+      <c r="F18" s="6">
+        <v>2.4</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="H18" s="15">
+        <f t="shared" si="0"/>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="12">
         <v>14</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="26" t="s">
         <v>33</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="6">
         <v>17</v>
       </c>
-      <c r="E19" s="18" t="s">
+      <c r="E19" s="20" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="15">
+      <c r="F19" s="6">
+        <f>2.67/20</f>
+        <v>0.13350000000000001</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="H19" s="15">
+        <f t="shared" si="0"/>
+        <v>2.2695000000000003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="12">
         <v>15</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="26" t="s">
         <v>33</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="6">
         <v>6</v>
       </c>
-      <c r="E20" s="18" t="s">
+      <c r="E20" s="20" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="15">
+      <c r="F20" s="6">
+        <f>2.63/20</f>
+        <v>0.13150000000000001</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="H20" s="15">
+        <f t="shared" si="0"/>
+        <v>0.78900000000000003</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="12">
         <v>16</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="26" t="s">
         <v>36</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="6">
         <v>2</v>
       </c>
-      <c r="E21" s="18" t="s">
+      <c r="E21" s="20" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="15">
+      <c r="F21" s="6"/>
+      <c r="G21" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="H21" s="15"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="12">
         <v>17</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="26" t="s">
         <v>37</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="6">
         <v>1</v>
       </c>
-      <c r="E22" s="18" t="s">
+      <c r="E22" s="20" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="15">
+      <c r="F22" s="6"/>
+      <c r="G22" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="H22" s="15"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="12">
         <v>18</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="26" t="s">
         <v>38</v>
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="6">
         <v>1</v>
       </c>
-      <c r="E23" s="18" t="s">
+      <c r="E23" s="20" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="15">
+      <c r="F23" s="6"/>
+      <c r="G23" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="H23" s="15"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="12">
         <v>19</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="26" t="s">
         <v>39</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="6">
         <v>1</v>
       </c>
-      <c r="E24" s="18" t="s">
+      <c r="E24" s="20" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="15">
+      <c r="F24" s="6">
+        <v>1.67</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="H24" s="15">
+        <f>D24*F24</f>
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="12">
         <v>20</v>
       </c>
-      <c r="B25" s="12" t="s">
+      <c r="B25" s="26" t="s">
         <v>41</v>
       </c>
       <c r="C25" s="6"/>
       <c r="D25" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="E25" s="18" t="s">
+      <c r="E25" s="20" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="15">
+      <c r="F25" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="H25" s="15"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="12">
         <v>21</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="B26" s="26" t="s">
         <v>46</v>
       </c>
       <c r="C26" s="6" t="s">
@@ -1296,15 +1565,20 @@
       <c r="D26" s="6">
         <v>2</v>
       </c>
-      <c r="E26" s="18" t="s">
+      <c r="E26" s="20" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="15">
+      <c r="F26" s="6"/>
+      <c r="G26" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="H26" s="15"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="12">
         <v>22</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B27" s="26" t="s">
         <v>47</v>
       </c>
       <c r="C27" s="6" t="s">
@@ -1313,15 +1587,20 @@
       <c r="D27" s="6">
         <v>1</v>
       </c>
-      <c r="E27" s="18" t="s">
+      <c r="E27" s="20" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="15">
+      <c r="F27" s="6"/>
+      <c r="G27" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="H27" s="15"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="12">
         <v>23</v>
       </c>
-      <c r="B28" s="12" t="s">
+      <c r="B28" s="26" t="s">
         <v>48</v>
       </c>
       <c r="C28" s="6" t="s">
@@ -1330,15 +1609,20 @@
       <c r="D28" s="6">
         <v>1</v>
       </c>
-      <c r="E28" s="18" t="s">
+      <c r="E28" s="20" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="15">
+      <c r="F28" s="6"/>
+      <c r="G28" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="H28" s="15"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="12">
         <v>24</v>
       </c>
-      <c r="B29" s="12" t="s">
+      <c r="B29" s="26" t="s">
         <v>51</v>
       </c>
       <c r="C29" s="6" t="s">
@@ -1347,191 +1631,273 @@
       <c r="D29" s="6">
         <v>1</v>
       </c>
-      <c r="E29" s="18" t="s">
+      <c r="E29" s="20" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="15">
+      <c r="F29" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="H29" s="15"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="12">
         <v>25</v>
       </c>
-      <c r="B30" s="12" t="s">
+      <c r="B30" s="26" t="s">
         <v>52</v>
       </c>
       <c r="C30" s="6"/>
       <c r="D30" s="6">
         <v>2</v>
       </c>
-      <c r="E30" s="18" t="s">
+      <c r="E30" s="20" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="15">
+      <c r="F30" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="H30" s="15"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="12">
         <v>26</v>
       </c>
-      <c r="B31" s="12" t="s">
+      <c r="B31" s="26" t="s">
         <v>55</v>
       </c>
       <c r="C31" s="6"/>
       <c r="D31" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E31" s="18" t="s">
+      <c r="E31" s="20" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="15">
+      <c r="F31" s="6"/>
+      <c r="G31" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="H31" s="15"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="12">
         <v>27</v>
       </c>
-      <c r="B32" s="12" t="s">
+      <c r="B32" s="26" t="s">
         <v>57</v>
       </c>
       <c r="C32" s="6"/>
       <c r="D32" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="E32" s="18" t="s">
+      <c r="E32" s="20" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="15">
+      <c r="F32" s="6"/>
+      <c r="G32" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="H32" s="15"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="12">
         <v>28</v>
       </c>
-      <c r="B33" s="12" t="s">
+      <c r="B33" s="26" t="s">
         <v>58</v>
       </c>
       <c r="C33" s="6"/>
       <c r="D33" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E33" s="18" t="s">
+      <c r="E33" s="20" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="15">
+      <c r="F33" s="6"/>
+      <c r="G33" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="H33" s="15"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="12">
         <v>29</v>
       </c>
-      <c r="B34" s="12" t="s">
+      <c r="B34" s="26" t="s">
         <v>59</v>
       </c>
       <c r="C34" s="6"/>
       <c r="D34" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E34" s="18" t="s">
+      <c r="E34" s="20" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="15">
+      <c r="F34" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="H34" s="15"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="12">
         <v>30</v>
       </c>
-      <c r="B35" s="12" t="s">
+      <c r="B35" s="26" t="s">
         <v>60</v>
       </c>
       <c r="C35" s="6"/>
       <c r="D35" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E35" s="18" t="s">
+      <c r="E35" s="20" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="15">
+      <c r="F35" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="H35" s="15"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="12">
         <v>31</v>
       </c>
-      <c r="B36" s="12"/>
+      <c r="B36" s="26"/>
       <c r="C36" s="6"/>
       <c r="D36" s="6"/>
-      <c r="E36" s="18"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="15">
+      <c r="E36" s="20"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="15"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="12">
         <v>32</v>
       </c>
-      <c r="B37" s="12"/>
+      <c r="B37" s="26"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
-      <c r="E37" s="18"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="15">
+      <c r="E37" s="20"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="15"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="12">
         <v>33</v>
       </c>
-      <c r="B38" s="12"/>
+      <c r="B38" s="26"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
-      <c r="E38" s="18"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="15">
+      <c r="E38" s="20"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="15"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="12">
         <v>34</v>
       </c>
-      <c r="B39" s="12"/>
+      <c r="B39" s="26"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
-      <c r="E39" s="18"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="15">
+      <c r="E39" s="20"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="15"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="12">
         <v>35</v>
       </c>
-      <c r="B40" s="12"/>
+      <c r="B40" s="26"/>
       <c r="C40" s="6"/>
       <c r="D40" s="6"/>
-      <c r="E40" s="18"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="15">
+      <c r="E40" s="20"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="15"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="12">
         <v>36</v>
       </c>
-      <c r="B41" s="12"/>
+      <c r="B41" s="26"/>
       <c r="C41" s="6"/>
       <c r="D41" s="6"/>
-      <c r="E41" s="18"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="15">
+      <c r="E41" s="20"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="15"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="12">
         <v>37</v>
       </c>
-      <c r="B42" s="12"/>
+      <c r="B42" s="26"/>
       <c r="C42" s="6"/>
       <c r="D42" s="6"/>
-      <c r="E42" s="18"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="15">
+      <c r="E42" s="20"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="15"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="12">
         <v>38</v>
       </c>
-      <c r="B43" s="12"/>
+      <c r="B43" s="26"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
-      <c r="E43" s="18"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="15">
+      <c r="E43" s="20"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="15"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="12">
         <v>39</v>
       </c>
-      <c r="B44" s="12"/>
+      <c r="B44" s="26"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
-      <c r="E44" s="18"/>
-    </row>
-    <row r="45" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="16">
+      <c r="E44" s="20"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="15"/>
+    </row>
+    <row r="45" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="13">
         <v>40</v>
       </c>
-      <c r="B45" s="19"/>
-      <c r="C45" s="20"/>
-      <c r="D45" s="20"/>
+      <c r="B45" s="27"/>
+      <c r="C45" s="16"/>
+      <c r="D45" s="16"/>
       <c r="E45" s="21"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F45" s="16"/>
+      <c r="G45" s="28"/>
+      <c r="H45" s="29"/>
+    </row>
+    <row r="46" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G46" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="H46" s="9">
+        <f>SUM(H6:H45)</f>
+        <v>37.388500000000008</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>70</v>
       </c>
@@ -1542,12 +1908,12 @@
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B50" s="22" t="s">
+      <c r="B50" s="17" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B51" s="22" t="s">
+      <c r="B51" s="17" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1562,21 +1928,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Asiakirja" ma:contentTypeID="0x010100288FF80C09CDD44CBEDCB6BDA3BB791A" ma:contentTypeVersion="3" ma:contentTypeDescription="Luo uusi asiakirja." ma:contentTypeScope="" ma:versionID="e4c01c7c4b2fa601b9adbc8cdf8d23de">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="da167cd1-d7a6-4338-bc63-7a91f955c7fa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="30409ac8fa297c07eb11085401007006" ns2:_="">
     <xsd:import namespace="da167cd1-d7a6-4338-bc63-7a91f955c7fa"/>
@@ -1714,31 +2065,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0738F08B-BAB3-4861-8EE3-0808A07B6694}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="da167cd1-d7a6-4338-bc63-7a91f955c7fa"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{884C2661-2447-498C-AC3E-3E7F14D4616E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CE5D208-A7B2-407E-BE4C-99D8E137B990}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1754,4 +2096,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{884C2661-2447-498C-AC3E-3E7F14D4616E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0738F08B-BAB3-4861-8EE3-0808A07B6694}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="da167cd1-d7a6-4338-bc63-7a91f955c7fa"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added pics from first full assembly and main.py that works with external power source (without laptop). updated materials list.
</commit_message>
<xml_diff>
--- a/materials.xlsx
+++ b/materials.xlsx
@@ -2,20 +2,20 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samik\Documents\Koulu\digitaalisen_valmistuksen_perusteet\group23\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71940496-3A5C-49BC-9770-DEA8F0B78090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9B72A51F-6948-481A-ACBC-F10007722067}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{206C7778-B294-4357-AFEA-16B3EFD6E54B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,180 +36,201 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="79">
   <si>
     <t>Materials</t>
   </si>
   <si>
+    <t>Group 23</t>
+  </si>
+  <si>
     <t>violent light-chasing alarm clock</t>
   </si>
   <si>
-    <t>Group 23</t>
+    <t>Updated:</t>
   </si>
   <si>
     <t>#</t>
   </si>
   <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Size (in materials)</t>
+  </si>
+  <si>
     <t>Quantity</t>
   </si>
   <si>
+    <t>Material / component specification</t>
+  </si>
+  <si>
+    <t>Cost per unit [€]</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>Total [€]</t>
+  </si>
+  <si>
+    <t>Frame plate v1</t>
+  </si>
+  <si>
+    <t>?? x ?? x ?? mm</t>
+  </si>
+  <si>
     <t>Plywood</t>
   </si>
   <si>
+    <t>mm3</t>
+  </si>
+  <si>
+    <t>Frame plate v2</t>
+  </si>
+  <si>
+    <t>Front wheel</t>
+  </si>
+  <si>
+    <t>35931.574 mm3</t>
+  </si>
+  <si>
+    <t>PLA</t>
+  </si>
+  <si>
+    <t>Front wheel bracket v1</t>
+  </si>
+  <si>
+    <t>9213.417 mm3</t>
+  </si>
+  <si>
+    <t>Front wheel bracket v2</t>
+  </si>
+  <si>
+    <t>9002.649 mm3</t>
+  </si>
+  <si>
+    <t>Microcontroller</t>
+  </si>
+  <si>
+    <t>Raspberry Pi Pico W</t>
+  </si>
+  <si>
+    <t>piece</t>
+  </si>
+  <si>
+    <t>Breadboard</t>
+  </si>
+  <si>
+    <t>Big</t>
+  </si>
+  <si>
+    <t>Small</t>
+  </si>
+  <si>
+    <t>Phototransistor</t>
+  </si>
+  <si>
+    <t>TEPT5700</t>
+  </si>
+  <si>
+    <t>Resistor</t>
+  </si>
+  <si>
+    <t>10k ohm</t>
+  </si>
+  <si>
+    <t>Gear motor</t>
+  </si>
+  <si>
+    <t>H-bridge</t>
+  </si>
+  <si>
+    <t>L293D</t>
+  </si>
+  <si>
+    <t>Microservo</t>
+  </si>
+  <si>
+    <t>MG90S</t>
+  </si>
+  <si>
+    <t>Jumper cable</t>
+  </si>
+  <si>
+    <t>Male-male</t>
+  </si>
+  <si>
+    <t>Male-female</t>
+  </si>
+  <si>
+    <t>Rear wheel</t>
+  </si>
+  <si>
+    <t>3 x AAA</t>
+  </si>
+  <si>
+    <t>Electrical tape</t>
+  </si>
+  <si>
+    <t>max. 1 roll :D</t>
+  </si>
+  <si>
+    <t>black and blue</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>(Printed rear wheel)</t>
+  </si>
+  <si>
+    <t>check from cad mm3</t>
+  </si>
+  <si>
+    <t>TPU</t>
+  </si>
+  <si>
+    <t>(Servo bracket)</t>
+  </si>
+  <si>
+    <t>(Hammer)</t>
+  </si>
+  <si>
+    <t>TPU??</t>
+  </si>
+  <si>
+    <t>Prototype frame</t>
+  </si>
+  <si>
     <t>??</t>
   </si>
   <si>
-    <t>PLA</t>
-  </si>
-  <si>
-    <t>Item</t>
-  </si>
-  <si>
-    <t>Material / component specification</t>
-  </si>
-  <si>
-    <t>Front wheel</t>
-  </si>
-  <si>
-    <t>check from cad mm3</t>
-  </si>
-  <si>
-    <t>Frame plate v2</t>
-  </si>
-  <si>
-    <t>Frame plate v1</t>
-  </si>
-  <si>
-    <t>?? x ?? x ?? mm</t>
-  </si>
-  <si>
-    <t>2 or 4 or how many :D</t>
-  </si>
-  <si>
-    <t>Front wheel bracket v1</t>
-  </si>
-  <si>
-    <t>Front wheel bracket v2</t>
-  </si>
-  <si>
-    <t>Raspberry Pi Pico W</t>
-  </si>
-  <si>
-    <t>Microcontroller</t>
-  </si>
-  <si>
-    <t>Size (in materials)</t>
-  </si>
-  <si>
-    <t>Breadboard</t>
-  </si>
-  <si>
-    <t>Big</t>
-  </si>
-  <si>
-    <t>Small</t>
-  </si>
-  <si>
-    <t>Phototransistor</t>
-  </si>
-  <si>
-    <t>TEPT5700</t>
-  </si>
-  <si>
-    <t>Resistor</t>
-  </si>
-  <si>
-    <t>10k ohm</t>
-  </si>
-  <si>
-    <t>Gear motor</t>
-  </si>
-  <si>
-    <t>H-bridge</t>
-  </si>
-  <si>
-    <t>L293D</t>
-  </si>
-  <si>
-    <t>Microservo</t>
-  </si>
-  <si>
-    <t>MG90S</t>
-  </si>
-  <si>
-    <t>Jumper cable</t>
-  </si>
-  <si>
-    <t>Male-male</t>
-  </si>
-  <si>
-    <t>Male-female</t>
-  </si>
-  <si>
-    <t>Rear wheel</t>
-  </si>
-  <si>
-    <t>(Schottky diode)</t>
-  </si>
-  <si>
-    <t>(Slide switch)</t>
-  </si>
-  <si>
-    <t>(Battery holder)</t>
-  </si>
-  <si>
-    <t>3 x AAA</t>
-  </si>
-  <si>
-    <t>Electrical tape</t>
-  </si>
-  <si>
-    <t>black and blue</t>
+    <t>Cardboard</t>
+  </si>
+  <si>
+    <t>Prototype wheels</t>
+  </si>
+  <si>
+    <t>0.33l soda cans</t>
+  </si>
+  <si>
+    <t>(Bolt)</t>
   </si>
   <si>
     <t>4??</t>
   </si>
   <si>
-    <t>max. 1 roll :D</t>
-  </si>
-  <si>
-    <t>TPU</t>
-  </si>
-  <si>
-    <t>(Printed rear wheel)</t>
-  </si>
-  <si>
-    <t>(Servo bracket)</t>
-  </si>
-  <si>
-    <t>(Hammer)</t>
-  </si>
-  <si>
-    <t>TPU??</t>
-  </si>
-  <si>
-    <t>Cardboard</t>
-  </si>
-  <si>
-    <t>Prototype frame</t>
-  </si>
-  <si>
-    <t>Prototype wheels</t>
-  </si>
-  <si>
-    <t>0.33l soda cans</t>
-  </si>
-  <si>
-    <t>Updated:</t>
-  </si>
-  <si>
-    <t>(Bolt)</t>
+    <t>M4 x ?? mm ??</t>
+  </si>
+  <si>
+    <t>(Nut)</t>
   </si>
   <si>
     <t>12??</t>
   </si>
   <si>
-    <t>(Nut)</t>
+    <t>M4??</t>
   </si>
   <si>
     <t>(Screw)</t>
@@ -221,31 +242,7 @@
     <t>(The rauta-/kuparilanka)</t>
   </si>
   <si>
-    <t>M4 x ?? mm ??</t>
-  </si>
-  <si>
-    <t>M4??</t>
-  </si>
-  <si>
-    <t>GEARMOTOR 200 RPM 3-6V DC (Adafruit 3777??)</t>
-  </si>
-  <si>
-    <t>link or something?? Markings on the bag??</t>
-  </si>
-  <si>
-    <t>?? Markings on the bag??</t>
-  </si>
-  <si>
-    <t>35931.574 mm3</t>
-  </si>
-  <si>
-    <t>9002.649 mm3</t>
-  </si>
-  <si>
-    <t>9213.417 mm3</t>
-  </si>
-  <si>
-    <t>?? Which one??</t>
+    <t>TOTAL</t>
   </si>
   <si>
     <t>(brackets for not yet implemented/ready components/materials)</t>
@@ -254,34 +251,28 @@
     <t>remember to add jumpers with power source</t>
   </si>
   <si>
-    <t>+ 3 male-female</t>
-  </si>
-  <si>
-    <t>+ 2 female-female</t>
-  </si>
-  <si>
-    <t>maybe</t>
-  </si>
-  <si>
-    <t>Unit</t>
-  </si>
-  <si>
-    <t>mm3</t>
-  </si>
-  <si>
-    <t>piece</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>Cost per unit [€]</t>
-  </si>
-  <si>
-    <t>Total [€]</t>
-  </si>
-  <si>
-    <t>TOTAL</t>
+    <t>these might be €/g also</t>
+  </si>
+  <si>
+    <t>GEARMOTOR 200 RPM 3-6V DC (Adafruit 3777)</t>
+  </si>
+  <si>
+    <t>thin white wheel 65mm (Adafruit 3763)</t>
+  </si>
+  <si>
+    <t>STPS3L60</t>
+  </si>
+  <si>
+    <t>Schottky diode</t>
+  </si>
+  <si>
+    <t>SPDT</t>
+  </si>
+  <si>
+    <t>Slide switch</t>
+  </si>
+  <si>
+    <t>Battery holder</t>
   </si>
 </sst>
 </file>
@@ -651,7 +642,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -675,8 +666,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
@@ -700,6 +689,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1019,10 +1012,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11BCCBEE-3478-41B5-8E92-3DF53108FB7E}">
-  <dimension ref="A1:H52"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1035,308 +1028,311 @@
     <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>1</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>54</v>
+        <v>3</v>
       </c>
       <c r="E3">
-        <v>250423</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>250427</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="18" t="s">
+      <c r="F5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="G5" s="23" t="s">
-        <v>75</v>
-      </c>
-      <c r="H5" s="24" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G5" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
         <v>1</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="D6" s="7">
+        <v>4</v>
+      </c>
+      <c r="E6" s="19" t="s">
         <v>14</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="19" t="s">
-        <v>5</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7" t="s">
-        <v>76</v>
+        <v>15</v>
       </c>
       <c r="H6" s="14"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>2</v>
       </c>
-      <c r="B7" s="26" t="s">
-        <v>12</v>
+      <c r="B7" s="24" t="s">
+        <v>16</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D7" s="6">
         <v>2</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6" t="s">
-        <v>76</v>
+        <v>15</v>
       </c>
       <c r="H7" s="15"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>3</v>
       </c>
-      <c r="B8" s="26" t="s">
-        <v>10</v>
+      <c r="B8" s="24" t="s">
+        <v>17</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>66</v>
+        <v>18</v>
       </c>
       <c r="D8" s="6">
         <v>2</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6" t="s">
-        <v>76</v>
+        <v>15</v>
       </c>
       <c r="H8" s="15"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <v>4</v>
       </c>
-      <c r="B9" s="26" t="s">
-        <v>16</v>
+      <c r="B9" s="24" t="s">
+        <v>20</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>68</v>
+        <v>21</v>
       </c>
       <c r="D9" s="6">
         <v>1</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="6" t="s">
-        <v>76</v>
+        <v>15</v>
       </c>
       <c r="H9" s="15"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <v>5</v>
       </c>
-      <c r="B10" s="26" t="s">
-        <v>17</v>
+      <c r="B10" s="24" t="s">
+        <v>22</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>67</v>
+        <v>23</v>
       </c>
       <c r="D10" s="6">
         <v>2</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="6" t="s">
-        <v>76</v>
+        <v>15</v>
       </c>
       <c r="H10" s="15"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <v>6</v>
       </c>
-      <c r="B11" s="26" t="s">
-        <v>19</v>
+      <c r="B11" s="24" t="s">
+        <v>24</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6">
         <v>1</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="F11" s="6">
         <v>8.11</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>77</v>
+        <v>26</v>
       </c>
       <c r="H11" s="15">
         <f>D11*F11</f>
         <v>8.11</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <v>7</v>
       </c>
-      <c r="B12" s="26" t="s">
-        <v>21</v>
+      <c r="B12" s="24" t="s">
+        <v>27</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="6">
         <v>1</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="F12" s="6">
         <v>5.35</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>77</v>
+        <v>26</v>
       </c>
       <c r="H12" s="15">
         <f t="shared" ref="H12:H20" si="0">D12*F12</f>
         <v>5.35</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <v>8</v>
       </c>
-      <c r="B13" s="26" t="s">
-        <v>21</v>
+      <c r="B13" s="24" t="s">
+        <v>27</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6">
         <v>1</v>
       </c>
       <c r="E13" s="20" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F13" s="6">
         <v>2.72</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>77</v>
+        <v>26</v>
       </c>
       <c r="H13" s="15">
         <f t="shared" si="0"/>
         <v>2.72</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>9</v>
       </c>
-      <c r="B14" s="26" t="s">
-        <v>24</v>
+      <c r="B14" s="24" t="s">
+        <v>30</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6">
         <v>2</v>
       </c>
       <c r="E14" s="20" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="F14" s="6">
         <v>0.46</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>77</v>
+        <v>26</v>
       </c>
       <c r="H14" s="15">
         <f t="shared" si="0"/>
         <v>0.92</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>10</v>
       </c>
-      <c r="B15" s="26" t="s">
-        <v>26</v>
+      <c r="B15" s="24" t="s">
+        <v>32</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="6">
         <v>2</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="F15" s="6">
         <v>0.24</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>77</v>
+        <v>26</v>
       </c>
       <c r="H15" s="15">
         <f t="shared" si="0"/>
         <v>0.48</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <v>11</v>
       </c>
-      <c r="B16" s="26" t="s">
-        <v>28</v>
+      <c r="B16" s="24" t="s">
+        <v>34</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6">
         <v>2</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="F16" s="6">
         <v>2.72</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>77</v>
+        <v>26</v>
       </c>
       <c r="H16" s="15">
         <f t="shared" si="0"/>
@@ -1347,21 +1343,21 @@
       <c r="A17" s="12">
         <v>12</v>
       </c>
-      <c r="B17" s="26" t="s">
-        <v>29</v>
+      <c r="B17" s="24" t="s">
+        <v>35</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="6">
         <v>1</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="F17" s="6">
         <v>7.24</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>77</v>
+        <v>26</v>
       </c>
       <c r="H17" s="15">
         <f t="shared" si="0"/>
@@ -1372,21 +1368,21 @@
       <c r="A18" s="12">
         <v>13</v>
       </c>
-      <c r="B18" s="26" t="s">
-        <v>31</v>
+      <c r="B18" s="24" t="s">
+        <v>37</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="6">
         <v>1</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="F18" s="6">
         <v>2.4</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>77</v>
+        <v>26</v>
       </c>
       <c r="H18" s="15">
         <f t="shared" si="0"/>
@@ -1397,22 +1393,22 @@
       <c r="A19" s="12">
         <v>14</v>
       </c>
-      <c r="B19" s="26" t="s">
-        <v>33</v>
+      <c r="B19" s="24" t="s">
+        <v>39</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="6">
         <v>17</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="F19" s="6">
         <f>2.67/20</f>
         <v>0.13350000000000001</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>77</v>
+        <v>26</v>
       </c>
       <c r="H19" s="15">
         <f t="shared" si="0"/>
@@ -1423,22 +1419,22 @@
       <c r="A20" s="12">
         <v>15</v>
       </c>
-      <c r="B20" s="26" t="s">
-        <v>33</v>
+      <c r="B20" s="24" t="s">
+        <v>39</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="6">
         <v>6</v>
       </c>
       <c r="E20" s="20" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="F20" s="6">
         <f>2.63/20</f>
         <v>0.13150000000000001</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>77</v>
+        <v>26</v>
       </c>
       <c r="H20" s="15">
         <f t="shared" si="0"/>
@@ -1449,81 +1445,96 @@
       <c r="A21" s="12">
         <v>16</v>
       </c>
-      <c r="B21" s="26" t="s">
-        <v>36</v>
+      <c r="B21" s="24" t="s">
+        <v>42</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="6">
         <v>2</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="F21" s="6"/>
+        <v>73</v>
+      </c>
+      <c r="F21" s="6">
+        <v>1.38</v>
+      </c>
       <c r="G21" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="H21" s="15"/>
+        <v>26</v>
+      </c>
+      <c r="H21" s="15">
+        <f>D21*F21</f>
+        <v>2.76</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
         <v>17</v>
       </c>
-      <c r="B22" s="26" t="s">
-        <v>37</v>
+      <c r="B22" s="24" t="s">
+        <v>75</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="6">
         <v>1</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="F22" s="6"/>
+        <v>74</v>
+      </c>
+      <c r="F22" s="6">
+        <v>0.39</v>
+      </c>
       <c r="G22" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="H22" s="15"/>
+        <v>26</v>
+      </c>
+      <c r="H22" s="15">
+        <f>D22*F22</f>
+        <v>0.39</v>
+      </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
         <v>18</v>
       </c>
-      <c r="B23" s="26" t="s">
-        <v>38</v>
+      <c r="B23" s="24" t="s">
+        <v>77</v>
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="6">
         <v>1</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="F23" s="6"/>
+        <v>76</v>
+      </c>
+      <c r="F23" s="6">
+        <v>0.88</v>
+      </c>
       <c r="G23" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="H23" s="15"/>
+        <v>26</v>
+      </c>
+      <c r="H23" s="15">
+        <f>D23*F23</f>
+        <v>0.88</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
         <v>19</v>
       </c>
-      <c r="B24" s="26" t="s">
-        <v>39</v>
+      <c r="B24" s="24" t="s">
+        <v>78</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="6">
         <v>1</v>
       </c>
       <c r="E24" s="20" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F24" s="6">
         <v>1.67</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>77</v>
+        <v>26</v>
       </c>
       <c r="H24" s="15">
         <f>D24*F24</f>
@@ -1534,21 +1545,21 @@
       <c r="A25" s="12">
         <v>20</v>
       </c>
-      <c r="B25" s="26" t="s">
-        <v>41</v>
+      <c r="B25" s="24" t="s">
+        <v>44</v>
       </c>
       <c r="C25" s="6"/>
       <c r="D25" s="6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E25" s="20" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="H25" s="15"/>
     </row>
@@ -1556,21 +1567,21 @@
       <c r="A26" s="12">
         <v>21</v>
       </c>
-      <c r="B26" s="26" t="s">
-        <v>46</v>
+      <c r="B26" s="24" t="s">
+        <v>48</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="D26" s="6">
         <v>2</v>
       </c>
       <c r="E26" s="20" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="F26" s="6"/>
       <c r="G26" s="6" t="s">
-        <v>76</v>
+        <v>15</v>
       </c>
       <c r="H26" s="15"/>
     </row>
@@ -1578,21 +1589,21 @@
       <c r="A27" s="12">
         <v>22</v>
       </c>
-      <c r="B27" s="26" t="s">
-        <v>47</v>
+      <c r="B27" s="24" t="s">
+        <v>51</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="D27" s="6">
         <v>1</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="F27" s="6"/>
       <c r="G27" s="6" t="s">
-        <v>76</v>
+        <v>15</v>
       </c>
       <c r="H27" s="15"/>
     </row>
@@ -1600,21 +1611,21 @@
       <c r="A28" s="12">
         <v>23</v>
       </c>
-      <c r="B28" s="26" t="s">
-        <v>48</v>
+      <c r="B28" s="24" t="s">
+        <v>52</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="D28" s="6">
         <v>1</v>
       </c>
       <c r="E28" s="20" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="F28" s="6"/>
       <c r="G28" s="6" t="s">
-        <v>76</v>
+        <v>15</v>
       </c>
       <c r="H28" s="15"/>
     </row>
@@ -1622,23 +1633,23 @@
       <c r="A29" s="12">
         <v>24</v>
       </c>
-      <c r="B29" s="26" t="s">
-        <v>51</v>
+      <c r="B29" s="24" t="s">
+        <v>54</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>6</v>
+        <v>55</v>
       </c>
       <c r="D29" s="6">
         <v>1</v>
       </c>
       <c r="E29" s="20" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="H29" s="15"/>
     </row>
@@ -1646,21 +1657,21 @@
       <c r="A30" s="12">
         <v>25</v>
       </c>
-      <c r="B30" s="26" t="s">
-        <v>52</v>
+      <c r="B30" s="24" t="s">
+        <v>57</v>
       </c>
       <c r="C30" s="6"/>
       <c r="D30" s="6">
         <v>2</v>
       </c>
       <c r="E30" s="20" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="H30" s="15"/>
     </row>
@@ -1668,19 +1679,19 @@
       <c r="A31" s="12">
         <v>26</v>
       </c>
-      <c r="B31" s="26" t="s">
-        <v>55</v>
+      <c r="B31" s="24" t="s">
+        <v>59</v>
       </c>
       <c r="C31" s="6"/>
       <c r="D31" s="6" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="E31" s="20" t="s">
         <v>61</v>
       </c>
       <c r="F31" s="6"/>
       <c r="G31" s="6" t="s">
-        <v>77</v>
+        <v>26</v>
       </c>
       <c r="H31" s="15"/>
     </row>
@@ -1688,19 +1699,19 @@
       <c r="A32" s="12">
         <v>27</v>
       </c>
-      <c r="B32" s="26" t="s">
-        <v>57</v>
+      <c r="B32" s="24" t="s">
+        <v>62</v>
       </c>
       <c r="C32" s="6"/>
       <c r="D32" s="6" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="E32" s="20" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F32" s="6"/>
       <c r="G32" s="6" t="s">
-        <v>77</v>
+        <v>26</v>
       </c>
       <c r="H32" s="15"/>
     </row>
@@ -1708,19 +1719,19 @@
       <c r="A33" s="12">
         <v>28</v>
       </c>
-      <c r="B33" s="26" t="s">
-        <v>58</v>
+      <c r="B33" s="24" t="s">
+        <v>65</v>
       </c>
       <c r="C33" s="6"/>
       <c r="D33" s="6" t="s">
-        <v>6</v>
+        <v>55</v>
       </c>
       <c r="E33" s="20" t="s">
-        <v>6</v>
+        <v>55</v>
       </c>
       <c r="F33" s="6"/>
       <c r="G33" s="6" t="s">
-        <v>77</v>
+        <v>26</v>
       </c>
       <c r="H33" s="15"/>
     </row>
@@ -1728,21 +1739,21 @@
       <c r="A34" s="12">
         <v>29</v>
       </c>
-      <c r="B34" s="26" t="s">
-        <v>59</v>
+      <c r="B34" s="24" t="s">
+        <v>66</v>
       </c>
       <c r="C34" s="6"/>
       <c r="D34" s="6" t="s">
-        <v>6</v>
+        <v>55</v>
       </c>
       <c r="E34" s="20" t="s">
-        <v>6</v>
+        <v>55</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="H34" s="15"/>
     </row>
@@ -1750,21 +1761,21 @@
       <c r="A35" s="12">
         <v>30</v>
       </c>
-      <c r="B35" s="26" t="s">
-        <v>60</v>
+      <c r="B35" s="24" t="s">
+        <v>67</v>
       </c>
       <c r="C35" s="6"/>
       <c r="D35" s="6" t="s">
-        <v>6</v>
+        <v>55</v>
       </c>
       <c r="E35" s="20" t="s">
-        <v>6</v>
+        <v>55</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="H35" s="15"/>
     </row>
@@ -1772,7 +1783,7 @@
       <c r="A36" s="12">
         <v>31</v>
       </c>
-      <c r="B36" s="26"/>
+      <c r="B36" s="24"/>
       <c r="C36" s="6"/>
       <c r="D36" s="6"/>
       <c r="E36" s="20"/>
@@ -1784,7 +1795,7 @@
       <c r="A37" s="12">
         <v>32</v>
       </c>
-      <c r="B37" s="26"/>
+      <c r="B37" s="24"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="20"/>
@@ -1796,7 +1807,7 @@
       <c r="A38" s="12">
         <v>33</v>
       </c>
-      <c r="B38" s="26"/>
+      <c r="B38" s="24"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="20"/>
@@ -1808,7 +1819,7 @@
       <c r="A39" s="12">
         <v>34</v>
       </c>
-      <c r="B39" s="26"/>
+      <c r="B39" s="24"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="20"/>
@@ -1820,7 +1831,7 @@
       <c r="A40" s="12">
         <v>35</v>
       </c>
-      <c r="B40" s="26"/>
+      <c r="B40" s="24"/>
       <c r="C40" s="6"/>
       <c r="D40" s="6"/>
       <c r="E40" s="20"/>
@@ -1832,7 +1843,7 @@
       <c r="A41" s="12">
         <v>36</v>
       </c>
-      <c r="B41" s="26"/>
+      <c r="B41" s="24"/>
       <c r="C41" s="6"/>
       <c r="D41" s="6"/>
       <c r="E41" s="20"/>
@@ -1844,7 +1855,7 @@
       <c r="A42" s="12">
         <v>37</v>
       </c>
-      <c r="B42" s="26"/>
+      <c r="B42" s="24"/>
       <c r="C42" s="6"/>
       <c r="D42" s="6"/>
       <c r="E42" s="20"/>
@@ -1856,7 +1867,7 @@
       <c r="A43" s="12">
         <v>38</v>
       </c>
-      <c r="B43" s="26"/>
+      <c r="B43" s="24"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="20"/>
@@ -1868,7 +1879,7 @@
       <c r="A44" s="12">
         <v>39</v>
       </c>
-      <c r="B44" s="26"/>
+      <c r="B44" s="24"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="20"/>
@@ -1880,47 +1891,38 @@
       <c r="A45" s="13">
         <v>40</v>
       </c>
-      <c r="B45" s="27"/>
+      <c r="B45" s="25"/>
       <c r="C45" s="16"/>
       <c r="D45" s="16"/>
       <c r="E45" s="21"/>
       <c r="F45" s="16"/>
-      <c r="G45" s="28"/>
-      <c r="H45" s="29"/>
+      <c r="G45" s="26"/>
+      <c r="H45" s="27"/>
     </row>
     <row r="46" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G46" s="30" t="s">
-        <v>81</v>
+      <c r="G46" s="28" t="s">
+        <v>68</v>
       </c>
       <c r="H46" s="9">
         <f>SUM(H6:H45)</f>
-        <v>37.388500000000008</v>
+        <v>41.418500000000009</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B50" s="17" t="s">
-        <v>72</v>
-      </c>
+      <c r="B50" s="17"/>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B51" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
-        <v>74</v>
-      </c>
+      <c r="B51" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1928,8 +1930,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Asiakirja" ma:contentTypeID="0x010100288FF80C09CDD44CBEDCB6BDA3BB791A" ma:contentTypeVersion="3" ma:contentTypeDescription="Luo uusi asiakirja." ma:contentTypeScope="" ma:versionID="e4c01c7c4b2fa601b9adbc8cdf8d23de">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="da167cd1-d7a6-4338-bc63-7a91f955c7fa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="30409ac8fa297c07eb11085401007006" ns2:_="">
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100288FF80C09CDD44CBEDCB6BDA3BB791A" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="daf59a59666b18c77d16c7900867ac2e">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="da167cd1-d7a6-4338-bc63-7a91f955c7fa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c8e8fbdc805c43d29a2e081e89408539" ns2:_="">
     <xsd:import namespace="da167cd1-d7a6-4338-bc63-7a91f955c7fa"/>
     <xsd:element name="properties">
       <xsd:complexType>
@@ -1975,8 +1986,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Sisältölaji"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Otsikko"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -2065,15 +2076,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2081,7 +2083,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CE5D208-A7B2-407E-BE4C-99D8E137B990}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{884C2661-2447-498C-AC3E-3E7F14D4616E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B7ED468-D2AB-4F3A-9751-48EE847F168E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
@@ -2098,26 +2108,18 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{884C2661-2447-498C-AC3E-3E7F14D4616E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0738F08B-BAB3-4861-8EE3-0808A07B6694}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="da167cd1-d7a6-4338-bc63-7a91f955c7fa"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated materials list and schematic
</commit_message>
<xml_diff>
--- a/materials.xlsx
+++ b/materials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samik\Documents\Koulu\digitaalisen_valmistuksen_perusteet\group23\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9B72A51F-6948-481A-ACBC-F10007722067}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8A8CFDF-FC9B-4F22-8694-0C672A92234E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{206C7778-B294-4357-AFEA-16B3EFD6E54B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="78">
   <si>
     <t>Materials</t>
   </si>
@@ -77,39 +77,21 @@
     <t>Frame plate v1</t>
   </si>
   <si>
-    <t>?? x ?? x ?? mm</t>
-  </si>
-  <si>
-    <t>Plywood</t>
-  </si>
-  <si>
-    <t>mm3</t>
-  </si>
-  <si>
     <t>Frame plate v2</t>
   </si>
   <si>
     <t>Front wheel</t>
   </si>
   <si>
-    <t>35931.574 mm3</t>
-  </si>
-  <si>
     <t>PLA</t>
   </si>
   <si>
     <t>Front wheel bracket v1</t>
   </si>
   <si>
-    <t>9213.417 mm3</t>
-  </si>
-  <si>
     <t>Front wheel bracket v2</t>
   </si>
   <si>
-    <t>9002.649 mm3</t>
-  </si>
-  <si>
     <t>Microcontroller</t>
   </si>
   <si>
@@ -173,21 +155,12 @@
     <t>Electrical tape</t>
   </si>
   <si>
-    <t>max. 1 roll :D</t>
-  </si>
-  <si>
-    <t>black and blue</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
     <t>(Printed rear wheel)</t>
   </si>
   <si>
-    <t>check from cad mm3</t>
-  </si>
-  <si>
     <t>TPU</t>
   </si>
   <si>
@@ -197,63 +170,24 @@
     <t>(Hammer)</t>
   </si>
   <si>
-    <t>TPU??</t>
-  </si>
-  <si>
     <t>Prototype frame</t>
   </si>
   <si>
     <t>??</t>
   </si>
   <si>
-    <t>Cardboard</t>
-  </si>
-  <si>
     <t>Prototype wheels</t>
   </si>
   <si>
-    <t>0.33l soda cans</t>
-  </si>
-  <si>
-    <t>(Bolt)</t>
-  </si>
-  <si>
-    <t>4??</t>
-  </si>
-  <si>
-    <t>M4 x ?? mm ??</t>
-  </si>
-  <si>
-    <t>(Nut)</t>
-  </si>
-  <si>
-    <t>12??</t>
-  </si>
-  <si>
-    <t>M4??</t>
-  </si>
-  <si>
     <t>(Screw)</t>
   </si>
   <si>
-    <t>(The nippuside)</t>
-  </si>
-  <si>
-    <t>(The rauta-/kuparilanka)</t>
-  </si>
-  <si>
     <t>TOTAL</t>
   </si>
   <si>
     <t>(brackets for not yet implemented/ready components/materials)</t>
   </si>
   <si>
-    <t>remember to add jumpers with power source</t>
-  </si>
-  <si>
-    <t>these might be €/g also</t>
-  </si>
-  <si>
     <t>GEARMOTOR 200 RPM 3-6V DC (Adafruit 3777)</t>
   </si>
   <si>
@@ -273,6 +207,69 @@
   </si>
   <si>
     <t>Battery holder</t>
+  </si>
+  <si>
+    <t>9213.417 mm3 / 9 g</t>
+  </si>
+  <si>
+    <t>9002.649 mm3 / 9 g</t>
+  </si>
+  <si>
+    <t>35931.574 mm3 / 28 g</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>Cable tie</t>
+  </si>
+  <si>
+    <t>(Steel wire)</t>
+  </si>
+  <si>
+    <t>M5 x 50 mm</t>
+  </si>
+  <si>
+    <t>M5</t>
+  </si>
+  <si>
+    <t>Washer</t>
+  </si>
+  <si>
+    <t>Nut</t>
+  </si>
+  <si>
+    <t>Bolt</t>
+  </si>
+  <si>
+    <t>PLA?</t>
+  </si>
+  <si>
+    <t>150 x 145 x 3 mm</t>
+  </si>
+  <si>
+    <t>135 x 65 x 3 mm</t>
+  </si>
+  <si>
+    <t>Plywood (thickness = 3 mm)</t>
+  </si>
+  <si>
+    <t>mm2</t>
+  </si>
+  <si>
+    <t>34516.570 mm3 / ?? g</t>
+  </si>
+  <si>
+    <t>30372.943 mm3 / ?? g</t>
+  </si>
+  <si>
+    <t>45181.519 mm3 / ?? g</t>
+  </si>
+  <si>
+    <t>Cardboard from recycling bin</t>
+  </si>
+  <si>
+    <t>0.33l recyclable soda cans</t>
   </si>
 </sst>
 </file>
@@ -689,10 +686,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1012,10 +1005,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11BCCBEE-3478-41B5-8E92-3DF53108FB7E}">
-  <dimension ref="A1:I51"/>
+  <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K34" sqref="K34"/>
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1028,17 +1021,17 @@
     <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
@@ -1046,11 +1039,11 @@
         <v>3</v>
       </c>
       <c r="E3">
-        <v>250427</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>250429</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>4</v>
       </c>
@@ -1076,7 +1069,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
         <v>1</v>
       </c>
@@ -1084,255 +1077,277 @@
         <v>12</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>13</v>
+        <v>70</v>
       </c>
       <c r="D6" s="7">
         <v>4</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="7"/>
+        <v>71</v>
+      </c>
+      <c r="F6" s="7">
+        <v>2.0999999999999999E-5</v>
+      </c>
       <c r="G6" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6" s="14"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="H6" s="14">
+        <f>F6*135*65*D6</f>
+        <v>0.73709999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>2</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="D7" s="6">
         <v>2</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="6"/>
+        <v>71</v>
+      </c>
+      <c r="F7" s="6">
+        <v>2.0999999999999999E-5</v>
+      </c>
       <c r="G7" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H7" s="15"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="H7" s="15">
+        <f>F7*150*145*D7</f>
+        <v>0.91349999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>3</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="D8" s="6">
         <v>2</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" s="6"/>
+        <v>15</v>
+      </c>
+      <c r="F8" s="6">
+        <v>1.4E-2</v>
+      </c>
       <c r="G8" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" s="15"/>
-      <c r="I8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="H8" s="15">
+        <f>F8*28*D8</f>
+        <v>0.78400000000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <v>4</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="D9" s="6">
         <v>1</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="6"/>
+        <v>15</v>
+      </c>
+      <c r="F9" s="6">
+        <v>1.4E-2</v>
+      </c>
       <c r="G9" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" s="15"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="H9" s="15">
+        <f>F9*9*D9</f>
+        <v>0.126</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <v>5</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="D10" s="6">
         <v>2</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" s="6"/>
+        <v>15</v>
+      </c>
+      <c r="F10" s="6">
+        <v>1.4E-2</v>
+      </c>
       <c r="G10" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H10" s="15"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="H10" s="15">
+        <f>F10*9*D10</f>
+        <v>0.252</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <v>6</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6">
         <v>1</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="F11" s="6">
         <v>8.11</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="H11" s="15">
         <f>D11*F11</f>
         <v>8.11</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <v>7</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="6">
         <v>1</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F12" s="6">
         <v>5.35</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="H12" s="15">
         <f t="shared" ref="H12:H20" si="0">D12*F12</f>
         <v>5.35</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <v>8</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6">
         <v>1</v>
       </c>
       <c r="E13" s="20" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F13" s="6">
         <v>2.72</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="H13" s="15">
         <f t="shared" si="0"/>
         <v>2.72</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>9</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6">
         <v>2</v>
       </c>
       <c r="E14" s="20" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="F14" s="6">
         <v>0.46</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="H14" s="15">
         <f t="shared" si="0"/>
         <v>0.92</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>10</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="6">
         <v>2</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F15" s="6">
         <v>0.24</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="H15" s="15">
         <f t="shared" si="0"/>
         <v>0.48</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <v>11</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6">
         <v>2</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="F16" s="6">
         <v>2.72</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="H16" s="15">
         <f t="shared" si="0"/>
@@ -1344,20 +1359,20 @@
         <v>12</v>
       </c>
       <c r="B17" s="24" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="6">
         <v>1</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F17" s="6">
         <v>7.24</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="H17" s="15">
         <f t="shared" si="0"/>
@@ -1369,20 +1384,20 @@
         <v>13</v>
       </c>
       <c r="B18" s="24" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="6">
         <v>1</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F18" s="6">
         <v>2.4</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="H18" s="15">
         <f t="shared" si="0"/>
@@ -1394,25 +1409,25 @@
         <v>14</v>
       </c>
       <c r="B19" s="24" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="6">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="F19" s="6">
         <f>2.67/20</f>
         <v>0.13350000000000001</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="H19" s="15">
         <f t="shared" si="0"/>
-        <v>2.2695000000000003</v>
+        <v>2.5365000000000002</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1420,25 +1435,25 @@
         <v>15</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="6">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E20" s="20" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="F20" s="6">
         <f>2.63/20</f>
         <v>0.13150000000000001</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="H20" s="15">
         <f t="shared" si="0"/>
-        <v>0.78900000000000003</v>
+        <v>1.052</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1446,20 +1461,20 @@
         <v>16</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="6">
         <v>2</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="F21" s="6">
         <v>1.38</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="H21" s="15">
         <f>D21*F21</f>
@@ -1471,20 +1486,20 @@
         <v>17</v>
       </c>
       <c r="B22" s="24" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="6">
         <v>1</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
       <c r="F22" s="6">
         <v>0.39</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="H22" s="15">
         <f>D22*F22</f>
@@ -1496,20 +1511,20 @@
         <v>18</v>
       </c>
       <c r="B23" s="24" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="6">
         <v>1</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="F23" s="6">
         <v>0.88</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="H23" s="15">
         <f>D23*F23</f>
@@ -1521,20 +1536,20 @@
         <v>19</v>
       </c>
       <c r="B24" s="24" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="6">
         <v>1</v>
       </c>
       <c r="E24" s="20" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="F24" s="6">
         <v>1.67</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="H24" s="15">
         <f>D24*F24</f>
@@ -1546,20 +1561,16 @@
         <v>20</v>
       </c>
       <c r="B25" s="24" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C25" s="6"/>
-      <c r="D25" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E25" s="20" t="s">
-        <v>46</v>
-      </c>
+      <c r="D25" s="6"/>
+      <c r="E25" s="20"/>
       <c r="F25" s="6" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="H25" s="15"/>
     </row>
@@ -1568,20 +1579,22 @@
         <v>21</v>
       </c>
       <c r="B26" s="24" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
       <c r="D26" s="6">
         <v>2</v>
       </c>
       <c r="E26" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="F26" s="6"/>
+        <v>41</v>
+      </c>
+      <c r="F26" s="6">
+        <v>4.9000000000000002E-2</v>
+      </c>
       <c r="G26" s="6" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="H26" s="15"/>
     </row>
@@ -1590,20 +1603,20 @@
         <v>22</v>
       </c>
       <c r="B27" s="24" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>49</v>
+        <v>74</v>
       </c>
       <c r="D27" s="6">
         <v>1</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="F27" s="6"/>
       <c r="G27" s="6" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="H27" s="15"/>
     </row>
@@ -1612,20 +1625,20 @@
         <v>23</v>
       </c>
       <c r="B28" s="24" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>49</v>
+        <v>75</v>
       </c>
       <c r="D28" s="6">
         <v>1</v>
       </c>
       <c r="E28" s="20" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="F28" s="6"/>
       <c r="G28" s="6" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="H28" s="15"/>
     </row>
@@ -1634,22 +1647,20 @@
         <v>24</v>
       </c>
       <c r="B29" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>55</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="C29" s="6"/>
       <c r="D29" s="6">
         <v>1</v>
       </c>
       <c r="E29" s="20" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="H29" s="15"/>
     </row>
@@ -1658,20 +1669,20 @@
         <v>25</v>
       </c>
       <c r="B30" s="24" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="C30" s="6"/>
       <c r="D30" s="6">
         <v>2</v>
       </c>
       <c r="E30" s="20" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="H30" s="15"/>
     </row>
@@ -1680,58 +1691,70 @@
         <v>26</v>
       </c>
       <c r="B31" s="24" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="C31" s="6"/>
-      <c r="D31" s="6" t="s">
-        <v>60</v>
+      <c r="D31" s="6">
+        <v>4</v>
       </c>
       <c r="E31" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="F31" s="6"/>
+        <v>63</v>
+      </c>
+      <c r="F31" s="6">
+        <f>0.99/10</f>
+        <v>9.9000000000000005E-2</v>
+      </c>
       <c r="G31" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="H31" s="15"/>
+        <v>20</v>
+      </c>
+      <c r="H31" s="15">
+        <f>F31*D31</f>
+        <v>0.39600000000000002</v>
+      </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
         <v>27</v>
       </c>
       <c r="B32" s="24" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C32" s="6"/>
-      <c r="D32" s="6" t="s">
-        <v>63</v>
+      <c r="D32" s="6">
+        <v>12</v>
       </c>
       <c r="E32" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="F32" s="6"/>
+      <c r="F32" s="6">
+        <f>2.99/25</f>
+        <v>0.11960000000000001</v>
+      </c>
       <c r="G32" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="H32" s="15"/>
+        <v>20</v>
+      </c>
+      <c r="H32" s="15">
+        <f>F32*D32</f>
+        <v>1.4352</v>
+      </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
         <v>28</v>
       </c>
       <c r="B33" s="24" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="C33" s="6"/>
       <c r="D33" s="6" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="E33" s="20" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="F33" s="6"/>
       <c r="G33" s="6" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="H33" s="15"/>
     </row>
@@ -1740,20 +1763,16 @@
         <v>29</v>
       </c>
       <c r="B34" s="24" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C34" s="6"/>
-      <c r="D34" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="E34" s="20" t="s">
-        <v>55</v>
-      </c>
+      <c r="D34" s="6"/>
+      <c r="E34" s="20"/>
       <c r="F34" s="6" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="H34" s="15"/>
     </row>
@@ -1762,20 +1781,16 @@
         <v>30</v>
       </c>
       <c r="B35" s="24" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C35" s="6"/>
-      <c r="D35" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="E35" s="20" t="s">
-        <v>55</v>
-      </c>
+      <c r="D35" s="6"/>
+      <c r="E35" s="20"/>
       <c r="F35" s="6" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="H35" s="15"/>
     </row>
@@ -1783,13 +1798,27 @@
       <c r="A36" s="12">
         <v>31</v>
       </c>
-      <c r="B36" s="24"/>
+      <c r="B36" s="24" t="s">
+        <v>65</v>
+      </c>
       <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="20"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="15"/>
+      <c r="D36" s="6">
+        <v>16</v>
+      </c>
+      <c r="E36" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="F36" s="6">
+        <f>2.99/25</f>
+        <v>0.11960000000000001</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H36" s="15">
+        <f>F36*D36</f>
+        <v>1.9136000000000002</v>
+      </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="12">
@@ -1901,21 +1930,16 @@
     </row>
     <row r="46" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G46" s="28" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="H46" s="9">
         <f>SUM(H6:H45)</f>
-        <v>41.418500000000009</v>
+        <v>48.505900000000011</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.25">
@@ -2111,15 +2135,15 @@
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0738F08B-BAB3-4861-8EE3-0808A07B6694}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="da167cd1-d7a6-4338-bc63-7a91f955c7fa"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="da167cd1-d7a6-4338-bc63-7a91f955c7fa"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated materials list & readme-file. added pics and demo video from final testing session & several versions of the final code (main_final.py is the one saved into the pico)
</commit_message>
<xml_diff>
--- a/materials.xlsx
+++ b/materials.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samik\Documents\Koulu\digitaalisen_valmistuksen_perusteet\group23\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8A8CFDF-FC9B-4F22-8694-0C672A92234E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1E3A6D0E-E1B0-4D12-909F-053164AFFDAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{206C7778-B294-4357-AFEA-16B3EFD6E54B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="80">
   <si>
     <t>Materials</t>
   </si>
@@ -158,18 +158,9 @@
     <t>-</t>
   </si>
   <si>
-    <t>(Printed rear wheel)</t>
-  </si>
-  <si>
     <t>TPU</t>
   </si>
   <si>
-    <t>(Servo bracket)</t>
-  </si>
-  <si>
-    <t>(Hammer)</t>
-  </si>
-  <si>
     <t>Prototype frame</t>
   </si>
   <si>
@@ -224,9 +215,6 @@
     <t>Cable tie</t>
   </si>
   <si>
-    <t>(Steel wire)</t>
-  </si>
-  <si>
     <t>M5 x 50 mm</t>
   </si>
   <si>
@@ -242,9 +230,6 @@
     <t>Bolt</t>
   </si>
   <si>
-    <t>PLA?</t>
-  </si>
-  <si>
     <t>150 x 145 x 3 mm</t>
   </si>
   <si>
@@ -257,19 +242,40 @@
     <t>mm2</t>
   </si>
   <si>
-    <t>34516.570 mm3 / ?? g</t>
-  </si>
-  <si>
-    <t>30372.943 mm3 / ?? g</t>
-  </si>
-  <si>
-    <t>45181.519 mm3 / ?? g</t>
-  </si>
-  <si>
     <t>Cardboard from recycling bin</t>
   </si>
   <si>
     <t>0.33l recyclable soda cans</t>
+  </si>
+  <si>
+    <t>45181.519 mm3 / 28 g</t>
+  </si>
+  <si>
+    <t>34516.570 mm3 / 18 g</t>
+  </si>
+  <si>
+    <t>30372.943 mm3 / 21 g</t>
+  </si>
+  <si>
+    <t>Printed rear wheel</t>
+  </si>
+  <si>
+    <t>Servo bracket</t>
+  </si>
+  <si>
+    <t>Hammer</t>
+  </si>
+  <si>
+    <t>Steel wire</t>
+  </si>
+  <si>
+    <t>Two-sided tape</t>
+  </si>
+  <si>
+    <t>FINAL ASSEMBLY</t>
+  </si>
+  <si>
+    <t>-final assembly includes for example only the printed rear wheels</t>
   </si>
 </sst>
 </file>
@@ -334,7 +340,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -635,11 +641,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -671,6 +703,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -686,6 +722,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1007,8 +1047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11BCCBEE-3478-41B5-8E92-3DF53108FB7E}">
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="J45" sqref="J45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1019,6 +1059,7 @@
     <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="43.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
@@ -1039,7 +1080,7 @@
         <v>3</v>
       </c>
       <c r="E3">
-        <v>250429</v>
+        <v>250503</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1077,19 +1118,19 @@
         <v>12</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D6" s="7">
         <v>4</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="F6" s="7">
         <v>2.0999999999999999E-5</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="H6" s="14">
         <f>F6*135*65*D6</f>
@@ -1104,19 +1145,19 @@
         <v>13</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D7" s="6">
         <v>2</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="F7" s="6">
         <v>2.0999999999999999E-5</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="H7" s="15">
         <f>F7*150*145*D7</f>
@@ -1131,7 +1172,7 @@
         <v>14</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D8" s="6">
         <v>2</v>
@@ -1143,7 +1184,7 @@
         <v>1.4E-2</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H8" s="15">
         <f>F8*28*D8</f>
@@ -1158,7 +1199,7 @@
         <v>16</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D9" s="6">
         <v>1</v>
@@ -1170,7 +1211,7 @@
         <v>1.4E-2</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H9" s="15">
         <f>F9*9*D9</f>
@@ -1185,7 +1226,7 @@
         <v>17</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D10" s="6">
         <v>2</v>
@@ -1197,7 +1238,7 @@
         <v>1.4E-2</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H10" s="15">
         <f>F10*9*D10</f>
@@ -1341,7 +1382,7 @@
         <v>2</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F16" s="6">
         <v>2.72</v>
@@ -1468,7 +1509,7 @@
         <v>2</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F21" s="6">
         <v>1.38</v>
@@ -1486,14 +1527,14 @@
         <v>17</v>
       </c>
       <c r="B22" s="24" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="6">
         <v>1</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F22" s="6">
         <v>0.39</v>
@@ -1511,14 +1552,14 @@
         <v>18</v>
       </c>
       <c r="B23" s="24" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="6">
         <v>1</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F23" s="6">
         <v>0.88</v>
@@ -1536,7 +1577,7 @@
         <v>19</v>
       </c>
       <c r="B24" s="24" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="6">
@@ -1579,82 +1620,95 @@
         <v>21</v>
       </c>
       <c r="B26" s="24" t="s">
-        <v>40</v>
+        <v>73</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D26" s="6">
         <v>2</v>
       </c>
       <c r="E26" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F26" s="6">
         <v>4.9000000000000002E-2</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="H26" s="15"/>
+        <v>57</v>
+      </c>
+      <c r="H26" s="15">
+        <f>F26*18*D26</f>
+        <v>1.764</v>
+      </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
         <v>22</v>
       </c>
       <c r="B27" s="24" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D27" s="6">
         <v>1</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="F27" s="6"/>
+        <v>15</v>
+      </c>
+      <c r="F27" s="6">
+        <v>1.4E-2</v>
+      </c>
       <c r="G27" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="H27" s="15"/>
+        <v>57</v>
+      </c>
+      <c r="H27" s="15">
+        <f>F27*21*D27</f>
+        <v>0.29399999999999998</v>
+      </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
         <v>23</v>
       </c>
       <c r="B28" s="24" t="s">
-        <v>43</v>
+        <v>75</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D28" s="6">
         <v>1</v>
       </c>
       <c r="E28" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="F28" s="6"/>
+        <v>15</v>
+      </c>
+      <c r="F28" s="6">
+        <v>1.4E-2</v>
+      </c>
       <c r="G28" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="H28" s="15"/>
+        <v>57</v>
+      </c>
+      <c r="H28" s="15">
+        <f>F28*28*D28</f>
+        <v>0.39200000000000002</v>
+      </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
         <v>24</v>
       </c>
       <c r="B29" s="24" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C29" s="6"/>
       <c r="D29" s="6">
         <v>1</v>
       </c>
       <c r="E29" s="20" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="F29" s="6" t="s">
         <v>39</v>
@@ -1669,14 +1723,14 @@
         <v>25</v>
       </c>
       <c r="B30" s="24" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C30" s="6"/>
       <c r="D30" s="6">
         <v>2</v>
       </c>
       <c r="E30" s="20" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="F30" s="6" t="s">
         <v>39</v>
@@ -1691,14 +1745,14 @@
         <v>26</v>
       </c>
       <c r="B31" s="24" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C31" s="6"/>
       <c r="D31" s="6">
         <v>4</v>
       </c>
       <c r="E31" s="20" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F31" s="6">
         <f>0.99/10</f>
@@ -1717,14 +1771,14 @@
         <v>27</v>
       </c>
       <c r="B32" s="24" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C32" s="6"/>
       <c r="D32" s="6">
         <v>12</v>
       </c>
       <c r="E32" s="20" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F32" s="6">
         <f>2.99/25</f>
@@ -1743,14 +1797,14 @@
         <v>28</v>
       </c>
       <c r="B33" s="24" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C33" s="6"/>
       <c r="D33" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E33" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F33" s="6"/>
       <c r="G33" s="6" t="s">
@@ -1763,7 +1817,7 @@
         <v>29</v>
       </c>
       <c r="B34" s="24" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
@@ -1781,7 +1835,7 @@
         <v>30</v>
       </c>
       <c r="B35" s="24" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
@@ -1799,14 +1853,14 @@
         <v>31</v>
       </c>
       <c r="B36" s="24" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C36" s="6"/>
       <c r="D36" s="6">
         <v>16</v>
       </c>
       <c r="E36" s="20" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F36" s="6">
         <f>2.99/25</f>
@@ -1824,12 +1878,18 @@
       <c r="A37" s="12">
         <v>32</v>
       </c>
-      <c r="B37" s="24"/>
+      <c r="B37" s="24" t="s">
+        <v>77</v>
+      </c>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="20"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
+      <c r="F37" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>39</v>
+      </c>
       <c r="H37" s="15"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -1929,23 +1989,35 @@
       <c r="H45" s="27"/>
     </row>
     <row r="46" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G46" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="H46" s="9">
+      <c r="G46" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="H46" s="30">
         <f>SUM(H6:H45)</f>
-        <v>48.505900000000011</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+        <v>50.955900000000014</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="G47" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="H47" s="9">
+        <f>SUM(H7,H8,H10,H11,H12,H13,H14,H15,H16,H17,H18,H19,H20,H22,H23,H24,H25,H26,H27,H28,H31,H32,H34,H35,H36,H37)</f>
+        <v>47.332800000000013</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G49" s="17" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="17"/>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B51" s="17"/>
     </row>
   </sheetData>
@@ -2135,15 +2207,15 @@
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0738F08B-BAB3-4861-8EE3-0808A07B6694}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="da167cd1-d7a6-4338-bc63-7a91f955c7fa"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="da167cd1-d7a6-4338-bc63-7a91f955c7fa"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>